<commit_message>
add 0926 flaw report
</commit_message>
<xml_diff>
--- a/Testing/0926-22.03xfce/0926-22.03xfce测试用例.xlsx
+++ b/Testing/0926-22.03xfce/0926-22.03xfce测试用例.xlsx
@@ -11,7 +11,7 @@
     <sheet name="测试用例" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">测试用例!$A$2:$N$52</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">测试用例!$A$2:$O$52</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="233">
   <si>
     <t xml:space="preserve">任务名称：</t>
   </si>
@@ -44,6 +44,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">测试</t>
     </r>
@@ -68,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">前置条件</t>
+  </si>
+  <si>
+    <t xml:space="preserve">环境配置</t>
   </si>
   <si>
     <t xml:space="preserve">操作步骤</t>
@@ -110,6 +114,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">基本使用</t>
     </r>
@@ -127,6 +132,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">使用</t>
     </r>
@@ -146,9 +152,14 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">镜像</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Archlinux 5.19.11-arch1-1
+QEMU emulator version 7.1.0</t>
   </si>
   <si>
     <t xml:space="preserve">启动虚拟机</t>
@@ -206,6 +217,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">设置</t>
     </r>
@@ -323,6 +335,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">自动隐藏</t>
     </r>
@@ -407,6 +420,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">桌面设置</t>
     </r>
@@ -590,6 +604,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">终端</t>
     </r>
@@ -860,6 +875,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">配置存储系统</t>
     </r>
@@ -879,7 +895,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -908,12 +924,7 @@
       <color rgb="FF000000"/>
       <name val="Source Han Sans CN"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Source Han Sans CN"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -979,7 +990,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1000,11 +1011,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1017,14 +1028,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1078,29 +1081,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="14.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="15" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="16" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1122,6 +1125,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -1166,7 +1170,9 @@
       <c r="N2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AMD2" s="0"/>
+      <c r="O2" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
       <c r="AMG2" s="0"/>
@@ -1179,77 +1185,81 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="H3" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="I3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="13" t="n">
+      <c r="L3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="11" t="n">
         <v>44832</v>
       </c>
-      <c r="N3" s="14" t="s">
-        <v>25</v>
+      <c r="O3" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="10" t="s">
-        <v>28</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="14" t="s">
         <v>32</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1257,377 +1267,388 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="10" t="s">
-        <v>38</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="10" t="s">
-        <v>49</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="14" t="s">
-        <v>40</v>
+        <v>52</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="10" t="s">
-        <v>54</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="14" t="s">
-        <v>40</v>
+        <v>57</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
       <c r="B9" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="10" t="s">
-        <v>59</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="14" t="s">
-        <v>40</v>
+        <v>62</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="10" t="s">
-        <v>64</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="14" t="s">
-        <v>40</v>
+        <v>67</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="10" t="s">
-        <v>69</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="14" t="s">
-        <v>40</v>
+        <v>72</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="10" t="s">
-        <v>73</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="14" t="s">
-        <v>40</v>
+        <v>76</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
       <c r="B13" s="9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="10" t="s">
-        <v>77</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="14" t="s">
-        <v>40</v>
+        <v>80</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
       <c r="B14" s="9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="10" t="s">
-        <v>81</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="14" t="s">
-        <v>40</v>
+        <v>85</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="14" t="s">
-        <v>40</v>
+      <c r="L15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1635,479 +1656,493 @@
         <v>3</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="10" t="s">
-        <v>90</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="9"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" s="9"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="14" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="10" t="s">
-        <v>98</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="14" t="s">
-        <v>91</v>
+        <v>101</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="9"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
       <c r="B19" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="10" t="s">
-        <v>102</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="14" t="s">
-        <v>91</v>
+        <v>105</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="10" t="s">
-        <v>106</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="14" t="s">
-        <v>91</v>
+        <v>109</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="9"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="10" t="s">
-        <v>110</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
       <c r="I21" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="14" t="s">
-        <v>91</v>
+        <v>113</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="10" t="s">
-        <v>114</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="14" t="s">
-        <v>91</v>
+        <v>117</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
       <c r="B23" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="10" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="10" t="s">
-        <v>118</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L23" s="9"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="14" t="s">
-        <v>91</v>
+        <v>121</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
       <c r="B24" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="10" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="10" t="s">
-        <v>122</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L24" s="9"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="14" t="s">
-        <v>91</v>
+        <v>125</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="9"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
       <c r="B25" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="10" t="s">
-        <v>126</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L25" s="9"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="14" t="s">
-        <v>91</v>
+        <v>129</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
       <c r="B26" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="10" t="s">
-        <v>130</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
       <c r="I26" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="14" t="s">
-        <v>91</v>
+        <v>133</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
       <c r="B27" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="10" t="s">
-        <v>134</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
       <c r="I27" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L27" s="9"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="14" t="s">
-        <v>91</v>
+        <v>137</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="9"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
       <c r="B28" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="10" t="s">
-        <v>138</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
       <c r="I28" s="10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L28" s="9"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14" t="s">
-        <v>91</v>
+        <v>141</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="9"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
       <c r="B29" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="J29" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>139</v>
-      </c>
       <c r="K29" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L29" s="9"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="14" t="s">
-        <v>91</v>
+        <v>141</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="9"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2115,207 +2150,213 @@
         <v>4</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="10" t="s">
-        <v>145</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
       <c r="I30" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="L30" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30" s="9"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="B31" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="L31" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="9"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="J31" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="K31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L31" s="9"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="14" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
       <c r="B32" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G32" s="11"/>
-      <c r="H32" s="10" t="s">
-        <v>153</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
       <c r="I32" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L32" s="9"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="14" t="s">
-        <v>146</v>
+        <v>156</v>
+      </c>
+      <c r="L32" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="9"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
       <c r="B33" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="G33" s="11"/>
-      <c r="H33" s="10" t="s">
-        <v>157</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
       <c r="I33" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L33" s="9"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="14" t="s">
-        <v>146</v>
+        <v>160</v>
+      </c>
+      <c r="L33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="9"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8"/>
       <c r="B34" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G34" s="11"/>
-      <c r="H34" s="10" t="s">
-        <v>161</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
       <c r="I34" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L34" s="9"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="14" t="s">
-        <v>146</v>
+        <v>164</v>
+      </c>
+      <c r="L34" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="9"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
       <c r="B35" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="G35" s="11"/>
-      <c r="H35" s="10" t="s">
-        <v>166</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
       <c r="I35" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L35" s="9"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="14" t="s">
-        <v>146</v>
+        <v>169</v>
+      </c>
+      <c r="L35" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M35" s="9"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2323,173 +2364,178 @@
         <v>5</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="10" t="s">
-        <v>170</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
       <c r="I36" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L36" s="9"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="14" t="s">
-        <v>171</v>
+        <v>172</v>
+      </c>
+      <c r="L36" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36" s="9"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="12" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8"/>
       <c r="B37" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C37" s="11"/>
+        <v>174</v>
+      </c>
+      <c r="C37" s="5"/>
       <c r="D37" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" s="9"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="K37" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L37" s="9"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="14" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
       <c r="B38" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C38" s="11"/>
+        <v>178</v>
+      </c>
+      <c r="C38" s="5"/>
       <c r="D38" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="J38" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>175</v>
-      </c>
       <c r="K38" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L38" s="9"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="14" t="s">
-        <v>171</v>
+        <v>177</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="9"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="12" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>
       <c r="B39" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C39" s="11"/>
+        <v>181</v>
+      </c>
+      <c r="C39" s="5"/>
       <c r="D39" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="G39" s="11"/>
-      <c r="H39" s="10" t="s">
-        <v>181</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
       <c r="I39" s="10" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L39" s="9"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="14" t="s">
-        <v>171</v>
+        <v>177</v>
+      </c>
+      <c r="L39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M39" s="9"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="12" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8"/>
       <c r="B40" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C40" s="11"/>
+        <v>184</v>
+      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="10" t="s">
-        <v>184</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
       <c r="I40" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L40" s="9"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="14" t="s">
-        <v>171</v>
+        <v>187</v>
+      </c>
+      <c r="L40" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M40" s="9"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="12" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2497,241 +2543,248 @@
         <v>6</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="G41" s="11"/>
-      <c r="H41" s="10" t="s">
-        <v>190</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
       <c r="I41" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L41" s="9"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="L41" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" s="9"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="12" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8"/>
       <c r="B42" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="J42" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="10" t="s">
+      <c r="K42" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42" s="9"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="12" t="s">
         <v>194</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="G42" s="11"/>
-      <c r="H42" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="J42" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="K42" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L42" s="9"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="14" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8"/>
       <c r="B43" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C43" s="11"/>
+        <v>198</v>
+      </c>
+      <c r="C43" s="5"/>
       <c r="D43" s="10" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="G43" s="11"/>
-      <c r="H43" s="10" t="s">
-        <v>198</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
       <c r="I43" s="10" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L43" s="9"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="L43" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M43" s="9"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="12" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8"/>
       <c r="B44" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C44" s="11"/>
+        <v>201</v>
+      </c>
+      <c r="C44" s="5"/>
       <c r="D44" s="10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="G44" s="11"/>
-      <c r="H44" s="10" t="s">
-        <v>201</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
       <c r="I44" s="10" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L44" s="9"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="L44" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" s="9"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="12" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8"/>
       <c r="B45" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C45" s="11"/>
+        <v>204</v>
+      </c>
+      <c r="C45" s="5"/>
       <c r="D45" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="10" t="s">
-        <v>204</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
       <c r="I45" s="10" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L45" s="9"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="L45" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M45" s="9"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="12" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8"/>
       <c r="B46" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C46" s="11"/>
+        <v>207</v>
+      </c>
+      <c r="C46" s="5"/>
       <c r="D46" s="10" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="G46" s="11"/>
-      <c r="H46" s="10" t="s">
-        <v>207</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
       <c r="I46" s="10" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L46" s="9"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="L46" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M46" s="9"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="12" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8"/>
       <c r="B47" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="C47" s="11"/>
+        <v>210</v>
+      </c>
+      <c r="C47" s="5"/>
       <c r="D47" s="10" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="G47" s="11"/>
-      <c r="H47" s="10" t="s">
-        <v>210</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
       <c r="I47" s="10" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L47" s="9"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="L47" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="9"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="12" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2739,223 +2792,194 @@
         <v>7</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>214</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="G48" s="11"/>
-      <c r="H48" s="10" t="s">
-        <v>213</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
       <c r="I48" s="10" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L48" s="9"/>
-      <c r="M48" s="13"/>
-      <c r="N48" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="L48" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" s="9"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="12" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8"/>
       <c r="B49" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C49" s="11"/>
+        <v>217</v>
+      </c>
+      <c r="C49" s="5"/>
       <c r="D49" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L49" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M49" s="9"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="12" t="s">
         <v>216</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="G49" s="11"/>
-      <c r="H49" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="J49" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="K49" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L49" s="9"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="14" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8"/>
       <c r="B50" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="C50" s="11"/>
+        <v>220</v>
+      </c>
+      <c r="C50" s="5"/>
       <c r="D50" s="10" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="G50" s="11"/>
-      <c r="H50" s="10" t="s">
-        <v>220</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
       <c r="I50" s="10" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L50" s="9"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="14" t="s">
-        <v>214</v>
+        <v>223</v>
+      </c>
+      <c r="L50" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="9"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="12" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8"/>
       <c r="B51" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C51" s="11"/>
+        <v>224</v>
+      </c>
+      <c r="C51" s="5"/>
       <c r="D51" s="10" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="G51" s="11"/>
-      <c r="H51" s="10" t="s">
-        <v>224</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
       <c r="I51" s="10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L51" s="9"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="14" t="s">
-        <v>214</v>
+        <v>228</v>
+      </c>
+      <c r="L51" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M51" s="9"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="12" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="14" t="n">
+      <c r="A52" s="12" t="n">
         <v>8</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>228</v>
+        <v>229</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>230</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="G52" s="11"/>
-      <c r="H52" s="10" t="s">
-        <v>229</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
       <c r="I52" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L52" s="9"/>
-      <c r="M52" s="13"/>
-      <c r="N52" s="14" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>231</v>
+      </c>
+      <c r="L52" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M52" s="9"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:N52"/>
-  <mergeCells count="18">
-    <mergeCell ref="B1:N1"/>
+  <autoFilter ref="A2:O52"/>
+  <mergeCells count="19">
+    <mergeCell ref="B1:O1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="G3:G52"/>
-    <mergeCell ref="L3:L52"/>
+    <mergeCell ref="H3:H52"/>
     <mergeCell ref="M3:M52"/>
+    <mergeCell ref="N3:N52"/>
     <mergeCell ref="A5:A15"/>
     <mergeCell ref="C5:C15"/>
     <mergeCell ref="A16:A29"/>
@@ -2978,7 +3002,7 @@
       <formula1>"高,中,低"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K52" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L2:L52" type="list">
       <formula1>"通过,不通过"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>